<commit_message>
Updated spec for bflc:*Statement properties.
</commit_message>
<xml_diff>
--- a/spec/ConvSpec-250-270-v2.1.xlsx
+++ b/spec/ConvSpec-250-270-v2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\share\BF 2.0 Bib specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\share\BF 2.0 Bib specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="148">
   <si>
     <t>250 - EDITION STATEMENT (R)</t>
   </si>
@@ -450,7 +450,19 @@
     <t xml:space="preserve">      $7 - Data provenance (R)</t>
   </si>
   <si>
-    <t>Fields 250-270 - Edition, Imprint, etc. - v2.0, 08/09/2022</t>
+    <t>Fields 250-270 - Edition, Imprint, etc. - v2.1, 10/04/2022</t>
+  </si>
+  <si>
+    <t>I - bflc:productionStatement ; concatenate $3, $a, $b, $c in order and retain (or reinsert) ISBD puntuation</t>
+  </si>
+  <si>
+    <t>I - bflc:publicationStatement ; concatenate $3, $a, $b, $c in order and retain (or reinsert) ISBD puntuation</t>
+  </si>
+  <si>
+    <t>I - bflc:distributionStatement ; concatenate $3, $a, $b, $c in order and retain (or reinsert) ISBD puntuation</t>
+  </si>
+  <si>
+    <t>I - bflc:manufactureStatement ; concatenate $3, $a, $b, $c in order and retain (or reinsert) ISBD puntuation</t>
   </si>
 </sst>
 </file>
@@ -889,15 +901,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="L114" sqref="L114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="8.7109375" style="2"/>
@@ -1704,36 +1716,48 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B114" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C114" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B115" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C115" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B116" s="10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C116" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B117" s="10" t="s">
         <v>113</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="63" x14ac:dyDescent="0.25">

</xml_diff>